<commit_message>
Change the salary structure.
</commit_message>
<xml_diff>
--- a/financial_stament.xlsx
+++ b/financial_stament.xlsx
@@ -38,159 +38,156 @@
     <t xml:space="preserve">Cost Level</t>
   </si>
   <si>
+    <t xml:space="preserve">High</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enter “High”, “Mid” or “Low”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Management Company</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Year 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Year 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Year 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BaseSalary+Benefits</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bonus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Paid From Performance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Payroll</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Technology+Equipment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marketing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ServiceProviders</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Real Estate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Furniture</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fund Expenses</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Legal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Portfolio Management System</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Order Management</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bloomberg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Refinitiv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Capital IQ, Factset</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Compute Cost</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quant Research Data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Intra Day Data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amazon Data Storage </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Audit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Administration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FinancialStatementPrep</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Director</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Virtual Secretary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grand Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Management Fees</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add a 75% buffer to management fees</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We are doing this to add a buffer in case our estimates are wrong and some fees spiral out of control</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AUM Needed for breakeven</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Strategy Returns Assumptions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Performance Share</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Performance </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Base Pay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Benefits</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Portfolio Manager</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quant Researcher</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quant Analyst</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Year 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ongoing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mid</t>
+  </si>
+  <si>
     <t xml:space="preserve">Low</t>
   </si>
   <si>
-    <t xml:space="preserve">Enter “High”, “Mid” or “Low”</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Management Company</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Year 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Year 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Year 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BaseSalary+Benefits</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bonus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Paid From Performance</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Payroll</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Technology+Equipment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Marketing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ServiceProviders</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Real Estate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Furniture</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fund Expenses</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Legal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Portfolio Management System</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Order Management</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bloomberg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Refinitiv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Capital IQ, Factset</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Compute Cost</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Quant Research Data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Intra Day Data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Amazon Data Storage </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Audit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Administration</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FinancialStatementPrep</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Director</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Virtual Secretary</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Grand Total</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Management Fees</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Add a 75% buffer to management fees</t>
-  </si>
-  <si>
-    <t xml:space="preserve">We are doing this to add a buffer in case our estimates are wrong and some fees spiral out of control</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AUM Needed for breakeven</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Strategy Returns Assumptions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Performance Share</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Performance </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Base Pay</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Benefits</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Portfolio Manager</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Trader</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Analyst</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Quant Analyst</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">High</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Year 0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ongoing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mid</t>
-  </si>
-  <si>
     <t xml:space="preserve">Number of Employees</t>
   </si>
   <si>
@@ -282,6 +279,9 @@
   </si>
   <si>
     <t xml:space="preserve">For Trader</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shared</t>
   </si>
   <si>
     <t xml:space="preserve">Monthly</t>
@@ -416,8 +416,8 @@
   </sheetPr>
   <dimension ref="A1:E50"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C29" activeCellId="0" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -467,16 +467,16 @@
         <v>8</v>
       </c>
       <c r="B7" s="1" t="n">
-        <f aca="false">Salary!D8</f>
-        <v>1105000</v>
+        <f aca="false">Salary!D7</f>
+        <v>500000</v>
       </c>
       <c r="C7" s="1" t="n">
         <f aca="false">B7*(1+$B$1)</f>
-        <v>1160250</v>
+        <v>525000</v>
       </c>
       <c r="D7" s="1" t="n">
         <f aca="false">C7*(1+$B$1)</f>
-        <v>1218262.5</v>
+        <v>551250</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -510,15 +510,15 @@
       </c>
       <c r="B10" s="1" t="n">
         <f aca="false">Tech_Equipment!B15</f>
-        <v>164500</v>
+        <v>87600</v>
       </c>
       <c r="C10" s="1" t="n">
         <f aca="false">Tech_Equipment!B12</f>
-        <v>149500</v>
+        <v>75600</v>
       </c>
       <c r="D10" s="1" t="n">
         <f aca="false">C10*(1+$B$1)</f>
-        <v>156975</v>
+        <v>79380</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -527,7 +527,7 @@
       </c>
       <c r="B11" s="3" t="n">
         <f aca="false">IF(B2="High", Marketing!B13, IF(B2="Low",Marketing!B38, IF(B2="Mid",Marketing!B26)))</f>
-        <v>42250</v>
+        <v>60500</v>
       </c>
       <c r="C11" s="1" t="n">
         <f aca="false">Marketing!B3</f>
@@ -544,15 +544,15 @@
       </c>
       <c r="B12" s="1" t="n">
         <f aca="false">IF(B2="High", ServiceProviders!D8, IF(B2="Low",ServiceProviders!D26, IF(B2="Mid",ServiceProviders!D17)))</f>
-        <v>91500</v>
+        <v>154000</v>
       </c>
       <c r="C12" s="1" t="n">
         <f aca="false">IF(B2="High", ServiceProviders!C8, IF(B2="Low",ServiceProviders!C26, IF(B2="Mid",ServiceProviders!C17)))</f>
-        <v>84000</v>
+        <v>144000</v>
       </c>
       <c r="D12" s="1" t="n">
         <f aca="false">C12*(1+$B$1)</f>
-        <v>88200</v>
+        <v>151200</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -561,15 +561,15 @@
       </c>
       <c r="B13" s="1" t="n">
         <f aca="false">IF(B2="High", RealEstate!B7, IF(B2="Low",RealEstate!B27, IF(B2="Mid",RealEstate!B16)))</f>
-        <v>37500</v>
+        <v>90000</v>
       </c>
       <c r="C13" s="1" t="n">
         <f aca="false">B13*(1+$B$1)</f>
-        <v>39375</v>
+        <v>94500</v>
       </c>
       <c r="D13" s="1" t="n">
         <f aca="false">C13*(1+$B$1)</f>
-        <v>41343.75</v>
+        <v>99225</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -583,15 +583,15 @@
       </c>
       <c r="B16" s="1" t="n">
         <f aca="false">SUM(B7:B13)</f>
-        <v>1441950</v>
+        <v>893300</v>
       </c>
       <c r="C16" s="1" t="n">
         <f aca="false">SUM(C7:C13)</f>
-        <v>1459385</v>
+        <v>865360</v>
       </c>
       <c r="D16" s="1" t="n">
         <f aca="false">SUM(D7:D13)</f>
-        <v>1532354.25</v>
+        <v>908628</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -605,15 +605,15 @@
       </c>
       <c r="B22" s="1" t="n">
         <f aca="false">IF(B2="High", Legal!B3, IF(B2="Mid",Legal!B8, IF(B2="Low",Legal!B13)))</f>
-        <v>65000</v>
+        <v>100000</v>
       </c>
       <c r="C22" s="1" t="n">
         <f aca="false">IF(B2="High", Legal!B4, IF(B2="Mid",Legal!B9, IF(B2="Low",Legal!B14)))</f>
-        <v>20000</v>
+        <v>50000</v>
       </c>
       <c r="D22" s="1" t="n">
         <f aca="false">C22*(1+$B$1)</f>
-        <v>21000</v>
+        <v>52500</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -622,15 +622,15 @@
       </c>
       <c r="B23" s="3" t="n">
         <f aca="false">IF(B2="High", PortfolioManagementSystem!B3, IF(B2="Mid",PortfolioManagementSystem!B14, IF(B2="Low",PortfolioManagementSystem!B26)))</f>
-        <v>50000</v>
+        <v>250000</v>
       </c>
       <c r="C23" s="1" t="n">
         <f aca="false">B23*(1+$B$1)</f>
-        <v>52500</v>
+        <v>262500</v>
       </c>
       <c r="D23" s="1" t="n">
         <f aca="false">C23*(1+$B$1)</f>
-        <v>55125</v>
+        <v>275625</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -639,15 +639,15 @@
       </c>
       <c r="B24" s="1" t="n">
         <f aca="false">IF(B2="High", PortfolioManagementSystem!B4, IF(B2="Mid",PortfolioManagementSystem!B15, IF(B2="Low",PortfolioManagementSystem!B27)))</f>
-        <v>20000</v>
+        <v>100000</v>
       </c>
       <c r="C24" s="1" t="n">
         <f aca="false">B24*(1+$B$1)</f>
-        <v>21000</v>
+        <v>105000</v>
       </c>
       <c r="D24" s="1" t="n">
         <f aca="false">C24*(1+$B$1)</f>
-        <v>22050</v>
+        <v>110250</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -702,10 +702,10 @@
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
+      <c r="A28" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B28" s="0" t="n">
+      <c r="B28" s="1" t="n">
         <v>50000</v>
       </c>
       <c r="C28" s="1" t="n">
@@ -718,10 +718,10 @@
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
+      <c r="A29" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B29" s="0" t="n">
+      <c r="B29" s="1" t="n">
         <v>200000</v>
       </c>
       <c r="C29" s="1" t="n">
@@ -734,10 +734,10 @@
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
+      <c r="A30" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B30" s="0" t="n">
+      <c r="B30" s="1" t="n">
         <v>100000</v>
       </c>
       <c r="C30" s="1" t="n">
@@ -750,10 +750,10 @@
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
+      <c r="A31" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B31" s="0" t="n">
+      <c r="B31" s="1" t="n">
         <v>5000</v>
       </c>
       <c r="C31" s="1" t="n">
@@ -771,15 +771,15 @@
       </c>
       <c r="B32" s="1" t="n">
         <f aca="false">IF(B2="High", Administration_Audit!C5, IF(B2="Mid",Administration_Audit!C15, IF(B2="Low",Administration_Audit!C25)))</f>
-        <v>65000</v>
+        <v>120000</v>
       </c>
       <c r="C32" s="1" t="n">
         <f aca="false">B32*(1+$B$1)</f>
-        <v>68250</v>
+        <v>126000</v>
       </c>
       <c r="D32" s="1" t="n">
         <f aca="false">C32*(1+$B$1)</f>
-        <v>71662.5</v>
+        <v>132300</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -788,15 +788,15 @@
       </c>
       <c r="B33" s="1" t="n">
         <f aca="false">IF(B2="High", Administration_Audit!D7, IF(B2="Mid",Administration_Audit!D17, IF(B2="Low",Administration_Audit!D27)))</f>
-        <v>132000</v>
+        <v>300000</v>
       </c>
       <c r="C33" s="1" t="n">
         <f aca="false">B33*(1+$B$1)</f>
-        <v>138600</v>
+        <v>315000</v>
       </c>
       <c r="D33" s="1" t="n">
         <f aca="false">C33*(1+$B$1)</f>
-        <v>145530</v>
+        <v>330750</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -805,15 +805,15 @@
       </c>
       <c r="B34" s="1" t="n">
         <f aca="false">IF(B2="High", Administration_Audit!C8, IF(B2="Mid",Administration_Audit!C18, IF(B2="Low",Administration_Audit!C28)))</f>
-        <v>10000</v>
+        <v>15000</v>
       </c>
       <c r="C34" s="1" t="n">
         <f aca="false">B34*(1+$B$1)</f>
-        <v>10500</v>
+        <v>15750</v>
       </c>
       <c r="D34" s="1" t="n">
         <f aca="false">C34*(1+$B$1)</f>
-        <v>11025</v>
+        <v>16537.5</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -822,15 +822,15 @@
       </c>
       <c r="B35" s="1" t="n">
         <f aca="false">IF(B2="High", Administration_Audit!C9, IF(B2="Mid",Administration_Audit!C19, IF(B2="Low",Administration_Audit!C29)))</f>
-        <v>0</v>
+        <v>20000</v>
       </c>
       <c r="C35" s="1" t="n">
         <f aca="false">B35*(1+$B$1)</f>
-        <v>0</v>
+        <v>21000</v>
       </c>
       <c r="D35" s="1" t="n">
         <f aca="false">C35*(1+$B$1)</f>
-        <v>0</v>
+        <v>22050</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -839,15 +839,15 @@
       </c>
       <c r="B36" s="1" t="n">
         <f aca="false">IF(B2="High", Administration_Audit!C10, IF(B2="Mid",Administration_Audit!C20, IF(B2="Low",Administration_Audit!C30)))</f>
-        <v>1000</v>
+        <v>3000</v>
       </c>
       <c r="C36" s="1" t="n">
         <f aca="false">B36*(1+$B$1)</f>
-        <v>1050</v>
+        <v>3150</v>
       </c>
       <c r="D36" s="1" t="n">
         <f aca="false">C36*(1+$B$1)</f>
-        <v>1102.5</v>
+        <v>3307.5</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -856,15 +856,15 @@
       </c>
       <c r="B38" s="1" t="n">
         <f aca="false">SUM(B22:B36)</f>
-        <v>741200</v>
+        <v>1306200</v>
       </c>
       <c r="C38" s="1" t="n">
         <f aca="false">SUM(C22:C36)</f>
-        <v>730010</v>
+        <v>1316510</v>
       </c>
       <c r="D38" s="1" t="n">
         <f aca="false">SUM(D22:D36)</f>
-        <v>766510.5</v>
+        <v>1382335.5</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -873,15 +873,15 @@
       </c>
       <c r="B41" s="4" t="n">
         <f aca="false">B16+B38</f>
-        <v>2183150</v>
+        <v>2199500</v>
       </c>
       <c r="C41" s="4" t="n">
         <f aca="false">C16+C38</f>
-        <v>2189395</v>
+        <v>2181870</v>
       </c>
       <c r="D41" s="4" t="n">
         <f aca="false">D16+D38</f>
-        <v>2298864.75</v>
+        <v>2290963.5</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -910,15 +910,15 @@
       </c>
       <c r="B45" s="4" t="n">
         <f aca="false">(B16+B38)/$B$44</f>
-        <v>191025625</v>
+        <v>192456250</v>
       </c>
       <c r="C45" s="4" t="n">
         <f aca="false">(C16+C38)/$B$44</f>
-        <v>191572062.5</v>
+        <v>190913625</v>
       </c>
       <c r="D45" s="4" t="n">
         <f aca="false">(D16+D38)/$B$44</f>
-        <v>201150665.625</v>
+        <v>200459306.25</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -949,15 +949,15 @@
       </c>
       <c r="B50" s="4" t="n">
         <f aca="false">(B48*B45)*$B$49</f>
-        <v>5730768.75</v>
+        <v>5773687.50000002</v>
       </c>
       <c r="C50" s="4" t="n">
         <f aca="false">(C48*C45)*$B$49</f>
-        <v>5747161.875</v>
+        <v>5727408.75000002</v>
       </c>
       <c r="D50" s="4" t="n">
         <f aca="false">(D48*D45)*$B$49</f>
-        <v>6034519.96875</v>
+        <v>6013779.18750002</v>
       </c>
     </row>
   </sheetData>
@@ -989,7 +989,7 @@
   <sheetData>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>49</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1062,7 +1062,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1135,7 +1135,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>2</v>
+        <v>51</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1222,54 +1222,89 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:B7"/>
+  <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="H22" activeCellId="0" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.53"/>
   </cols>
   <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="B2" s="1" t="n">
         <v>50000</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="1" t="n">
         <v>200000</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="1" t="n">
         <v>100000</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="0" t="n">
+      <c r="B5" s="1" t="n">
         <v>5000</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="0" t="n">
+      <c r="B7" s="1" t="n">
         <f aca="false">SUM(B2:B5)</f>
         <v>355000</v>
       </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="1"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="1"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="1"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="1"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="1"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="1"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="1"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B22" s="1"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B23" s="1"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1287,10 +1322,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:D11"/>
+  <dimension ref="A2:D10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1311,7 +1346,7 @@
         <v>44</v>
       </c>
       <c r="B3" s="1" t="n">
-        <v>275000</v>
+        <v>100000</v>
       </c>
       <c r="C3" s="1" t="n">
         <v>25000</v>
@@ -1322,7 +1357,7 @@
         <v>45</v>
       </c>
       <c r="B4" s="1" t="n">
-        <v>180000</v>
+        <v>100000</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>25000</v>
@@ -1333,7 +1368,7 @@
         <v>46</v>
       </c>
       <c r="B5" s="1" t="n">
-        <v>175000</v>
+        <v>100000</v>
       </c>
       <c r="C5" s="1" t="n">
         <v>25000</v>
@@ -1344,7 +1379,7 @@
         <v>47</v>
       </c>
       <c r="B6" s="1" t="n">
-        <v>175000</v>
+        <v>100000</v>
       </c>
       <c r="C6" s="1" t="n">
         <v>25000</v>
@@ -1352,34 +1387,23 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>48</v>
+        <v>17</v>
       </c>
       <c r="B7" s="1" t="n">
-        <v>175000</v>
+        <f aca="false">SUM(B3:B6)</f>
+        <v>400000</v>
       </c>
       <c r="C7" s="1" t="n">
-        <v>25000</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" s="1" t="n">
-        <f aca="false">SUM(B3:B7)</f>
-        <v>980000</v>
-      </c>
-      <c r="C8" s="1" t="n">
-        <f aca="false">SUM(C3:C7)</f>
-        <v>125000</v>
-      </c>
-      <c r="D8" s="1" t="n">
-        <f aca="false">B8+C8</f>
-        <v>1105000</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
+        <f aca="false">SUM(C3:C6)</f>
+        <v>100000</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <f aca="false">B7+C7</f>
+        <v>500000</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1442,7 +1466,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>49</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1452,7 +1476,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B3" s="1" t="n">
         <v>100000</v>
@@ -1460,7 +1484,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B4" s="1" t="n">
         <v>50000</v>
@@ -1468,7 +1492,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1478,7 +1502,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B8" s="1" t="n">
         <v>80000</v>
@@ -1486,7 +1510,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B9" s="1" t="n">
         <v>35000</v>
@@ -1494,7 +1518,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>2</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1504,7 +1528,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B13" s="1" t="n">
         <v>65000</v>
@@ -1512,7 +1536,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B14" s="1" t="n">
         <v>20000</v>
@@ -1537,7 +1561,7 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1547,21 +1571,21 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B2" s="1" t="n">
-        <f aca="false">COUNTA(Salary!A3:A7)</f>
-        <v>5</v>
+        <f aca="false">COUNTA(Salary!A3:A6)</f>
+        <v>4</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B3" s="1" t="n">
         <v>3000</v>
@@ -1570,34 +1594,34 @@
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="1" t="n">
         <f aca="false">B2*B3</f>
-        <v>15000</v>
+        <v>12000</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B7" s="1" t="n">
         <f aca="false">1000*B2</f>
-        <v>5000</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B8" s="1" t="n">
-        <v>15000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B9" s="1" t="n">
         <v>2500</v>
@@ -1605,7 +1629,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B10" s="1" t="n">
         <v>7200</v>
@@ -1613,7 +1637,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B11" s="1" t="n">
         <v>200</v>
@@ -1622,7 +1646,7 @@
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="1" t="n">
         <f aca="false">SUM($B$7:$B$11)*B$2</f>
-        <v>149500</v>
+        <v>75600</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1631,7 +1655,7 @@
       </c>
       <c r="B15" s="1" t="n">
         <f aca="false">B4+B12</f>
-        <v>164500</v>
+        <v>87600</v>
       </c>
     </row>
   </sheetData>
@@ -1663,18 +1687,18 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B1" s="1" t="n">
         <v>100</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B2" s="1" t="n">
         <v>250</v>
@@ -1682,7 +1706,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B3" s="1" t="n">
         <f aca="false">B2*B1</f>
@@ -1691,12 +1715,12 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>49</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B7" s="1" t="n">
         <v>30000</v>
@@ -1704,7 +1728,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B8" s="1" t="n">
         <v>2500</v>
@@ -1712,7 +1736,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B9" s="1" t="n">
         <v>500</v>
@@ -1720,7 +1744,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B10" s="1" t="n">
         <v>2500</v>
@@ -1743,12 +1767,12 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B20" s="1" t="n">
         <v>20000</v>
@@ -1756,7 +1780,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B21" s="1" t="n">
         <v>1500</v>
@@ -1764,7 +1788,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B22" s="1" t="n">
         <v>300</v>
@@ -1772,7 +1796,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B23" s="1" t="n">
         <v>1500</v>
@@ -1795,12 +1819,12 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>2</v>
+        <v>51</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B32" s="1" t="n">
         <v>15000</v>
@@ -1808,7 +1832,7 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B33" s="1" t="n">
         <v>1000</v>
@@ -1816,7 +1840,7 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B34" s="1" t="n">
         <v>250</v>
@@ -1824,7 +1848,7 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B35" s="1" t="n">
         <v>1000</v>
@@ -1871,15 +1895,15 @@
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>49</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>70</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>17</v>
@@ -1887,7 +1911,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B4" s="1" t="n">
         <v>3000</v>
@@ -1902,7 +1926,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B5" s="1" t="n">
         <v>3000</v>
@@ -1917,7 +1941,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B6" s="1" t="n">
         <v>4000</v>
@@ -1942,15 +1966,15 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>70</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>17</v>
@@ -1958,7 +1982,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B13" s="1" t="n">
         <v>3000</v>
@@ -1973,7 +1997,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B14" s="1" t="n">
         <v>3000</v>
@@ -1988,7 +2012,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B15" s="1" t="n">
         <v>4000</v>
@@ -2013,15 +2037,15 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>2</v>
+        <v>51</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>70</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>17</v>
@@ -2029,7 +2053,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B22" s="1" t="n">
         <v>2500</v>
@@ -2044,7 +2068,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B23" s="1" t="n">
         <v>2500</v>
@@ -2059,7 +2083,7 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B24" s="1" t="n">
         <v>2500</v>
@@ -2111,32 +2135,32 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B3" s="1" t="n">
         <v>300</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B4" s="1" t="n">
-        <f aca="false">COUNTA(Salary!$A$3:$A$7)*$B$3</f>
-        <v>1500</v>
+        <f aca="false">COUNTA(Salary!$A$3:$A$6)*$B$3</f>
+        <v>1200</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B5" s="1" t="n">
         <v>75</v>
@@ -2153,37 +2177,37 @@
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="1" t="n">
         <f aca="false">B5*B4</f>
-        <v>112500</v>
+        <v>90000</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B12" s="1" t="n">
         <v>200</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B13" s="1" t="n">
-        <f aca="false">COUNTA(Salary!$A$3:$A$7)*B12</f>
-        <v>1000</v>
+        <f aca="false">COUNTA(Salary!$A$3:$A$6)*B12</f>
+        <v>800</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B14" s="1" t="n">
         <v>60</v>
@@ -2200,37 +2224,37 @@
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="1" t="n">
         <f aca="false">B14*B13</f>
-        <v>60000</v>
+        <v>48000</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>2</v>
+        <v>51</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B23" s="1" t="n">
         <v>150</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B24" s="1" t="n">
-        <f aca="false">COUNTA(Salary!$A$3:$A$7)*B23</f>
-        <v>750</v>
+        <f aca="false">COUNTA(Salary!$A$3:$A$6)*B23</f>
+        <v>600</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B25" s="1" t="n">
         <v>50</v>
@@ -2247,7 +2271,7 @@
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="1" t="n">
         <f aca="false">B25*B24</f>
-        <v>37500</v>
+        <v>30000</v>
       </c>
     </row>
   </sheetData>
@@ -2269,7 +2293,7 @@
   <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2279,7 +2303,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>49</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2300,14 +2324,14 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B5" s="1" t="n">
+        <f aca="false">COUNTA(Salary!$A$3)*1900*12</f>
+        <v>22800</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>79</v>
-      </c>
-      <c r="B5" s="1" t="n">
-        <f aca="false">COUNTA(Salary!$A$3:$A$4)*1900*12</f>
-        <v>45600</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2319,7 +2343,7 @@
         <v>12000</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2331,18 +2355,18 @@
         <v>8400</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="1" t="n">
         <f aca="false">SUM(B3:B7)</f>
-        <v>416000</v>
+        <v>393200</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2363,14 +2387,14 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B16" s="1" t="n">
         <f aca="false">COUNTA(Salary!$A$3)*1900*12</f>
         <v>22800</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2382,7 +2406,7 @@
         <v>12000</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2394,7 +2418,7 @@
         <v>8400</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2405,7 +2429,7 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>2</v>
+        <v>51</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2426,7 +2450,7 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B28" s="1" t="n">
         <f aca="false">COUNTA(Salary!$A$3)*1900*12</f>
@@ -2445,7 +2469,7 @@
         <v>12000</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2457,7 +2481,7 @@
         <v>8400</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>